<commit_message>
complete system no noise
</commit_message>
<xml_diff>
--- a/predict/recorded_audios/report_photos/report.xlsx
+++ b/predict/recorded_audios/report_photos/report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D22"/>
+  <dimension ref="A2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,10 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>mean_amplitude</t>
+          <t>max_local_amplitude</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>max_local_amplitude</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>file_name</t>
         </is>
@@ -457,321 +452,235 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.17387580871582</v>
+        <v>1.954366445541382</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02164341769704299</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.14223960488354</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.04589070007205009</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413455.wav</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.228359699249268</v>
+        <v>2.959033727645874</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02471137347139211</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.2046319471134352</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.05773304402828217</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413460.wav</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.798452615737915</v>
+        <v>3.962219476699829</v>
       </c>
       <c r="B5" t="n">
-        <v>0.03994292452978898</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2603063323712693</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.04831305518746376</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914134713.wav</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.844629526138306</v>
+        <v>4.9663405418396</v>
       </c>
       <c r="B6" t="n">
-        <v>0.164227618688002</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.109313011797691</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.0461459681391716</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914134816.wav</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.298367500305176</v>
+        <v>5.969293832778931</v>
       </c>
       <c r="B7" t="n">
-        <v>0.02236706722227257</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.1539094649141905</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.04763097316026688</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914134914.wav</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6.802687168121338</v>
+        <v>6.971488237380981</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01389396198428149</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.149130760305391</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.1183869242668152</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413509.wav</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6.842530012130737</v>
+        <v>7.97303318977356</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1042427311658853</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.12938070219099</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.1052666828036308</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413518.wav</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8.305583238601685</v>
+        <v>8.974731683731079</v>
       </c>
       <c r="B10" t="n">
-        <v>0.01901678168651123</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.1939791721051867</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.0661206841468811</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413529.wav</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9.822811841964722</v>
+        <v>9.977128982543945</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1559626512611536</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.065236184868914</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.05795527622103691</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191413530.wav</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9.861629009246826</v>
+        <v>10.97979760169983</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0392523462882985</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.220034697827063</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.05269449204206467</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135410.wav</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11.30545830726624</v>
+        <v>11.98143911361694</v>
       </c>
       <c r="B13" t="n">
-        <v>0.02760246525906837</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.3015053438961882</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.09235147386789322</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135514.wav</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12.80779051780701</v>
+        <v>12.98377537727356</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1573224419755927</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1.072173383239574</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.07962875068187714</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135610.wav</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12.84927439689636</v>
+        <v>13.98786497116089</v>
       </c>
       <c r="B15" t="n">
-        <v>0.02231756468256525</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.4084042825039333</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.05643543228507042</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135719.wav</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14.32550120353699</v>
+        <v>14.9930534362793</v>
       </c>
       <c r="B16" t="n">
-        <v>0.01922189112514617</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.1161787112409208</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.0741506814956665</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135810.wav</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15.80837559700012</v>
+        <v>15.99627375602722</v>
       </c>
       <c r="B17" t="n">
-        <v>0.09662894368718003</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.9088684995407023</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.06636484712362289</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/2021051914135917.wav</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15.84406185150146</v>
+        <v>17.00104832649231</v>
       </c>
       <c r="B18" t="n">
-        <v>0.02309319111274652</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.1886548951649145</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.09688328206539154</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191414004.wav</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17.30964231491089</v>
+        <v>18.00464606285095</v>
       </c>
       <c r="B19" t="n">
-        <v>0.05769856854656422</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.997878414941765</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.08851940184831619</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191414017.wav</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18.81141662597656</v>
+        <v>19.00777387619019</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1024804401538221</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1.06366396820259</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>18.8539092540741</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.01951799694345461</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.09976886355206904</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>20.31298112869263</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.2064293189672545</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1.09959294928672</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>('/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/202104252055563.wav', 'wb')</t>
+        <v>0.127306342124939</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>/home/minhair/Desktop/food_ordering_system/food_ordering_system/predict/recorded_audios/environment_noise/202105191414025.wav</t>
         </is>
       </c>
     </row>

</xml_diff>